<commit_message>
Updated tables with different denominator for cc analysis
</commit_message>
<xml_diff>
--- a/aim1_table5_PP.xlsx
+++ b/aim1_table5_PP.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11610" firstSheet="2" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11610"/>
   </bookViews>
   <sheets>
     <sheet name="aim1_table5_PP" sheetId="1" r:id="rId1"/>
@@ -1188,7 +1188,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J23"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="K25" sqref="K24:K25"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
@@ -1296,28 +1298,28 @@
         <v>15</v>
       </c>
       <c r="C7">
-        <v>6469</v>
+        <v>5272</v>
       </c>
       <c r="D7">
-        <v>76.400000000000006</v>
+        <v>72.5</v>
       </c>
       <c r="E7">
-        <v>2683</v>
+        <v>2188</v>
       </c>
       <c r="F7">
         <v>41.5</v>
       </c>
       <c r="G7">
-        <v>673</v>
+        <v>583</v>
       </c>
       <c r="H7">
-        <v>10.4</v>
+        <v>11.1</v>
       </c>
       <c r="I7">
-        <v>3113</v>
+        <v>2501</v>
       </c>
       <c r="J7">
-        <v>48.1</v>
+        <v>47.4</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.35">
@@ -1328,7 +1330,7 @@
         <v>1996</v>
       </c>
       <c r="D8">
-        <v>23.6</v>
+        <v>27.5</v>
       </c>
       <c r="E8">
         <v>453</v>
@@ -1354,28 +1356,28 @@
         <v>24</v>
       </c>
       <c r="C9">
-        <v>8465</v>
+        <v>7268</v>
       </c>
       <c r="D9">
         <v>100</v>
       </c>
       <c r="E9">
-        <v>3136</v>
+        <v>2641</v>
       </c>
       <c r="F9">
-        <v>37</v>
+        <v>36.299999999999997</v>
       </c>
       <c r="G9">
-        <v>1277</v>
+        <v>1187</v>
       </c>
       <c r="H9">
-        <v>15.1</v>
+        <v>16.3</v>
       </c>
       <c r="I9">
-        <v>4052</v>
+        <v>3440</v>
       </c>
       <c r="J9">
-        <v>47.9</v>
+        <v>47.3</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.35">
@@ -1388,22 +1390,22 @@
         <v>15</v>
       </c>
       <c r="C11">
-        <v>2944</v>
+        <v>2545</v>
       </c>
       <c r="D11">
-        <v>75.2</v>
+        <v>72.400000000000006</v>
       </c>
       <c r="E11">
-        <v>2300</v>
+        <v>1983</v>
       </c>
       <c r="F11">
-        <v>78.099999999999994</v>
+        <v>77.900000000000006</v>
       </c>
       <c r="G11">
-        <v>644</v>
+        <v>562</v>
       </c>
       <c r="H11">
-        <v>21.9</v>
+        <v>22.1</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.35">
@@ -1414,7 +1416,7 @@
         <v>972</v>
       </c>
       <c r="D12">
-        <v>24.8</v>
+        <v>27.6</v>
       </c>
       <c r="E12">
         <v>400</v>
@@ -1434,22 +1436,22 @@
         <v>24</v>
       </c>
       <c r="C13">
-        <v>3916</v>
+        <v>3517</v>
       </c>
       <c r="D13">
         <v>100</v>
       </c>
       <c r="E13">
-        <v>2700</v>
+        <v>2383</v>
       </c>
       <c r="F13">
-        <v>68.900000000000006</v>
+        <v>67.8</v>
       </c>
       <c r="G13">
-        <v>1216</v>
+        <v>1134</v>
       </c>
       <c r="H13">
-        <v>31.1</v>
+        <v>32.200000000000003</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.35">
@@ -1619,7 +1621,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J23"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M16" sqref="M16"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
@@ -1727,28 +1731,28 @@
         <v>15</v>
       </c>
       <c r="C7">
-        <v>1547</v>
+        <v>1250</v>
       </c>
       <c r="D7">
-        <v>83.7</v>
+        <v>80.599999999999994</v>
       </c>
       <c r="E7">
-        <v>1277</v>
+        <v>1040</v>
       </c>
       <c r="F7">
-        <v>82.5</v>
+        <v>83.2</v>
       </c>
       <c r="G7">
-        <v>105</v>
+        <v>93</v>
       </c>
       <c r="H7">
-        <v>6.8</v>
+        <v>7.4</v>
       </c>
       <c r="I7">
-        <v>165</v>
+        <v>117</v>
       </c>
       <c r="J7">
-        <v>10.7</v>
+        <v>9.4</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.35">
@@ -1759,7 +1763,7 @@
         <v>301</v>
       </c>
       <c r="D8">
-        <v>16.3</v>
+        <v>19.399999999999999</v>
       </c>
       <c r="E8">
         <v>141</v>
@@ -1785,28 +1789,28 @@
         <v>24</v>
       </c>
       <c r="C9">
-        <v>1848</v>
+        <v>1551</v>
       </c>
       <c r="D9">
         <v>100</v>
       </c>
       <c r="E9">
-        <v>1418</v>
+        <v>1181</v>
       </c>
       <c r="F9">
-        <v>76.7</v>
+        <v>76.099999999999994</v>
       </c>
       <c r="G9">
-        <v>239</v>
+        <v>227</v>
       </c>
       <c r="H9">
-        <v>12.9</v>
+        <v>14.6</v>
       </c>
       <c r="I9">
-        <v>191</v>
+        <v>143</v>
       </c>
       <c r="J9">
-        <v>10.3</v>
+        <v>9.1999999999999993</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.35">
@@ -1819,22 +1823,22 @@
         <v>15</v>
       </c>
       <c r="C11">
-        <v>1242</v>
+        <v>1074</v>
       </c>
       <c r="D11">
-        <v>82.5</v>
+        <v>80.3</v>
       </c>
       <c r="E11">
-        <v>1138</v>
+        <v>982</v>
       </c>
       <c r="F11">
-        <v>91.6</v>
+        <v>91.4</v>
       </c>
       <c r="G11">
-        <v>104</v>
+        <v>92</v>
       </c>
       <c r="H11">
-        <v>8.4</v>
+        <v>8.6</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.35">
@@ -1845,7 +1849,7 @@
         <v>263</v>
       </c>
       <c r="D12">
-        <v>17.5</v>
+        <v>19.7</v>
       </c>
       <c r="E12">
         <v>129</v>
@@ -1865,22 +1869,22 @@
         <v>24</v>
       </c>
       <c r="C13">
-        <v>1505</v>
+        <v>1337</v>
       </c>
       <c r="D13">
         <v>100</v>
       </c>
       <c r="E13">
-        <v>1267</v>
+        <v>1111</v>
       </c>
       <c r="F13">
-        <v>84.2</v>
+        <v>83.1</v>
       </c>
       <c r="G13">
-        <v>238</v>
+        <v>226</v>
       </c>
       <c r="H13">
-        <v>15.8</v>
+        <v>16.899999999999999</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.35">
@@ -2050,7 +2054,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J23"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J14" sqref="J14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
@@ -2158,28 +2164,28 @@
         <v>15</v>
       </c>
       <c r="C7">
-        <v>2429</v>
+        <v>2024</v>
       </c>
       <c r="D7">
-        <v>72.3</v>
+        <v>68.5</v>
       </c>
       <c r="E7">
-        <v>920</v>
+        <v>778</v>
       </c>
       <c r="F7">
-        <v>37.9</v>
+        <v>38.4</v>
       </c>
       <c r="G7">
-        <v>307</v>
+        <v>265</v>
       </c>
       <c r="H7">
-        <v>12.6</v>
+        <v>13.1</v>
       </c>
       <c r="I7">
-        <v>1202</v>
+        <v>981</v>
       </c>
       <c r="J7">
-        <v>49.5</v>
+        <v>48.5</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.35">
@@ -2190,7 +2196,7 @@
         <v>929</v>
       </c>
       <c r="D8">
-        <v>27.7</v>
+        <v>31.5</v>
       </c>
       <c r="E8">
         <v>228</v>
@@ -2216,28 +2222,28 @@
         <v>24</v>
       </c>
       <c r="C9">
-        <v>3358</v>
+        <v>2953</v>
       </c>
       <c r="D9">
         <v>100</v>
       </c>
       <c r="E9">
-        <v>1148</v>
+        <v>1006</v>
       </c>
       <c r="F9">
-        <v>34.200000000000003</v>
+        <v>34.1</v>
       </c>
       <c r="G9">
-        <v>598</v>
+        <v>556</v>
       </c>
       <c r="H9">
-        <v>17.8</v>
+        <v>18.8</v>
       </c>
       <c r="I9">
-        <v>1612</v>
+        <v>1391</v>
       </c>
       <c r="J9">
-        <v>48</v>
+        <v>47.1</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.35">
@@ -2250,22 +2256,22 @@
         <v>15</v>
       </c>
       <c r="C11">
-        <v>1077</v>
+        <v>951</v>
       </c>
       <c r="D11">
-        <v>69</v>
+        <v>66.3</v>
       </c>
       <c r="E11">
-        <v>780</v>
+        <v>692</v>
       </c>
       <c r="F11">
-        <v>72.400000000000006</v>
+        <v>72.8</v>
       </c>
       <c r="G11">
-        <v>297</v>
+        <v>259</v>
       </c>
       <c r="H11">
-        <v>27.6</v>
+        <v>27.2</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.35">
@@ -2276,7 +2282,7 @@
         <v>484</v>
       </c>
       <c r="D12">
-        <v>31</v>
+        <v>33.700000000000003</v>
       </c>
       <c r="E12">
         <v>203</v>
@@ -2296,22 +2302,22 @@
         <v>24</v>
       </c>
       <c r="C13">
-        <v>1561</v>
+        <v>1435</v>
       </c>
       <c r="D13">
         <v>100</v>
       </c>
       <c r="E13">
-        <v>983</v>
+        <v>895</v>
       </c>
       <c r="F13">
-        <v>63</v>
+        <v>62.4</v>
       </c>
       <c r="G13">
-        <v>578</v>
+        <v>540</v>
       </c>
       <c r="H13">
-        <v>37</v>
+        <v>37.6</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.35">
@@ -2481,7 +2487,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J23"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M13" sqref="M13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
@@ -2589,28 +2597,28 @@
         <v>15</v>
       </c>
       <c r="C7">
-        <v>2493</v>
+        <v>1998</v>
       </c>
       <c r="D7">
-        <v>76.5</v>
+        <v>72.3</v>
       </c>
       <c r="E7">
-        <v>486</v>
+        <v>370</v>
       </c>
       <c r="F7">
-        <v>19.5</v>
+        <v>18.5</v>
       </c>
       <c r="G7">
-        <v>261</v>
+        <v>225</v>
       </c>
       <c r="H7">
-        <v>10.5</v>
+        <v>11.3</v>
       </c>
       <c r="I7">
-        <v>1746</v>
+        <v>1403</v>
       </c>
       <c r="J7">
-        <v>70</v>
+        <v>70.2</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.35">
@@ -2621,7 +2629,7 @@
         <v>766</v>
       </c>
       <c r="D8">
-        <v>23.5</v>
+        <v>27.7</v>
       </c>
       <c r="E8">
         <v>84</v>
@@ -2647,25 +2655,25 @@
         <v>24</v>
       </c>
       <c r="C9">
-        <v>3259</v>
+        <v>2764</v>
       </c>
       <c r="D9">
         <v>100</v>
       </c>
       <c r="E9">
-        <v>570</v>
+        <v>454</v>
       </c>
       <c r="F9">
-        <v>17.5</v>
+        <v>16.399999999999999</v>
       </c>
       <c r="G9">
-        <v>440</v>
+        <v>404</v>
       </c>
       <c r="H9">
-        <v>13.5</v>
+        <v>14.6</v>
       </c>
       <c r="I9">
-        <v>2249</v>
+        <v>1906</v>
       </c>
       <c r="J9">
         <v>69</v>
@@ -2681,22 +2689,22 @@
         <v>15</v>
       </c>
       <c r="C11">
-        <v>625</v>
+        <v>520</v>
       </c>
       <c r="D11">
-        <v>73.5</v>
+        <v>69.8</v>
       </c>
       <c r="E11">
-        <v>382</v>
+        <v>309</v>
       </c>
       <c r="F11">
-        <v>61.1</v>
+        <v>59.4</v>
       </c>
       <c r="G11">
-        <v>243</v>
+        <v>211</v>
       </c>
       <c r="H11">
-        <v>38.9</v>
+        <v>40.6</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.35">
@@ -2707,7 +2715,7 @@
         <v>225</v>
       </c>
       <c r="D12">
-        <v>26.5</v>
+        <v>30.2</v>
       </c>
       <c r="E12">
         <v>68</v>
@@ -2727,22 +2735,22 @@
         <v>24</v>
       </c>
       <c r="C13">
-        <v>850</v>
+        <v>745</v>
       </c>
       <c r="D13">
         <v>100</v>
       </c>
       <c r="E13">
-        <v>450</v>
+        <v>377</v>
       </c>
       <c r="F13">
-        <v>52.9</v>
+        <v>50.6</v>
       </c>
       <c r="G13">
-        <v>400</v>
+        <v>368</v>
       </c>
       <c r="H13">
-        <v>47.1</v>
+        <v>49.4</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.35">
@@ -2912,7 +2920,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J17" sqref="J17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
@@ -3020,28 +3030,28 @@
         <v>15</v>
       </c>
       <c r="C7">
-        <v>3976</v>
+        <v>3274</v>
       </c>
       <c r="D7">
-        <v>76.400000000000006</v>
+        <v>72.7</v>
       </c>
       <c r="E7">
-        <v>2197</v>
+        <v>1818</v>
       </c>
       <c r="F7">
-        <v>55.3</v>
+        <v>55.5</v>
       </c>
       <c r="G7">
-        <v>412</v>
+        <v>358</v>
       </c>
       <c r="H7">
-        <v>10.4</v>
+        <v>10.9</v>
       </c>
       <c r="I7">
-        <v>1367</v>
+        <v>1098</v>
       </c>
       <c r="J7">
-        <v>34.4</v>
+        <v>33.5</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.35">
@@ -3052,7 +3062,7 @@
         <v>1230</v>
       </c>
       <c r="D8">
-        <v>23.6</v>
+        <v>27.3</v>
       </c>
       <c r="E8">
         <v>369</v>
@@ -3078,28 +3088,28 @@
         <v>24</v>
       </c>
       <c r="C9">
-        <v>5206</v>
+        <v>4504</v>
       </c>
       <c r="D9">
         <v>100</v>
       </c>
       <c r="E9">
-        <v>2566</v>
+        <v>2187</v>
       </c>
       <c r="F9">
-        <v>49.3</v>
+        <v>48.6</v>
       </c>
       <c r="G9">
-        <v>837</v>
+        <v>783</v>
       </c>
       <c r="H9">
-        <v>16.100000000000001</v>
+        <v>17.399999999999999</v>
       </c>
       <c r="I9">
-        <v>1803</v>
+        <v>1534</v>
       </c>
       <c r="J9">
-        <v>34.6</v>
+        <v>34.1</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.35">
@@ -3112,19 +3122,19 @@
         <v>15</v>
       </c>
       <c r="C11">
-        <v>2319</v>
+        <v>2025</v>
       </c>
       <c r="D11">
-        <v>75.599999999999994</v>
+        <v>73.099999999999994</v>
       </c>
       <c r="E11">
-        <v>1918</v>
+        <v>1674</v>
       </c>
       <c r="F11">
         <v>82.7</v>
       </c>
       <c r="G11">
-        <v>401</v>
+        <v>351</v>
       </c>
       <c r="H11">
         <v>17.3</v>
@@ -3138,7 +3148,7 @@
         <v>747</v>
       </c>
       <c r="D12">
-        <v>24.4</v>
+        <v>26.9</v>
       </c>
       <c r="E12">
         <v>332</v>
@@ -3158,22 +3168,22 @@
         <v>24</v>
       </c>
       <c r="C13">
-        <v>3066</v>
+        <v>2772</v>
       </c>
       <c r="D13">
         <v>100</v>
       </c>
       <c r="E13">
-        <v>2250</v>
+        <v>2006</v>
       </c>
       <c r="F13">
-        <v>73.400000000000006</v>
+        <v>72.400000000000006</v>
       </c>
       <c r="G13">
-        <v>816</v>
+        <v>766</v>
       </c>
       <c r="H13">
-        <v>26.6</v>
+        <v>27.6</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.35">

</xml_diff>